<commit_message>
cleaning a dummy xlsx file using pandas
</commit_message>
<xml_diff>
--- a/codebase/extracted_polycab1.xlsx
+++ b/codebase/extracted_polycab1.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,452 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sr
+No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Item Code</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>HSN Code</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Supplier
+Item</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Delivery
+Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Qty</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>UOM</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr"/>
+      <c r="L1" s="1" t="inlineStr"/>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C-ADSF00096</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SAFETY CHEMICAL GOGGLES</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>90039000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NOS</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Note For Supplier:</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Project Number : Task Number : Expenditure Type :
+Expenditure Org :</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Unit Code : HALOL UH10-LAN CABLE-37A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ship To Location
+HALOL UH10-LAN CABLE-37A NEW R S NO 61,64 RAMPURA-KOTA MAIDA ROAD,
+VILLLAGE : RAMPURA, TALUKA : HALOL,DISTRICT : PANCHMAHALS HALOL
+GUJARAT IN 389350</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>21-JUN-
+25</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CGST-Slab 2
+SGST-Slab 2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>:
+:</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>39.00
+39.00</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Total Line Tax INR : 78.00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Total Line Amount INR : 728.00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Total PO Value INR : 728.00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Above materials should be supplied as per our purchase specifications
+Please also mention the P.O No. in all the future Correspondence.
+Taxes are indicatory and will be applicable as per norms at receipt.
+Supplier Note :</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Other Terms and Conditions :</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>SAFETY CHEMICAL GOGGLES</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Payment Terms</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>100% payment to be done on 60th day from the date of receipt of the material at stores</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Freight Terms</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DELIVERY/INCO Terms</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Destination</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Transporter</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>